<commit_message>
modified several tex files shifted to usenix style
</commit_message>
<xml_diff>
--- a/paper/figs/results.xlsx
+++ b/paper/figs/results.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22624"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="1340" yWindow="340" windowWidth="25520" windowHeight="15820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
   <si>
     <t>Internal Mode</t>
   </si>
@@ -77,6 +77,18 @@
   </si>
   <si>
     <t>External</t>
+  </si>
+  <si>
+    <t>PipeSize</t>
+  </si>
+  <si>
+    <t>Delay in Seconds</t>
+  </si>
+  <si>
+    <t>Application</t>
+  </si>
+  <si>
+    <t>Typical request size</t>
   </si>
 </sst>
 </file>
@@ -946,11 +958,11 @@
             </a:ln>
           </c:spPr>
         </c:serLines>
-        <c:axId val="2095414200"/>
-        <c:axId val="2095417176"/>
+        <c:axId val="2123902184"/>
+        <c:axId val="2119826936"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2095414200"/>
+        <c:axId val="2123902184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -989,7 +1001,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2095417176"/>
+        <c:crossAx val="2119826936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -997,7 +1009,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2095417176"/>
+        <c:axId val="2119826936"/>
         <c:scaling>
           <c:logBase val="10.0"/>
           <c:orientation val="minMax"/>
@@ -1038,7 +1050,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2095414200"/>
+        <c:crossAx val="2123902184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1776,11 +1788,11 @@
         </c:dLbls>
         <c:gapWidth val="0"/>
         <c:overlap val="100"/>
-        <c:axId val="2095526376"/>
-        <c:axId val="2095529352"/>
+        <c:axId val="2124016232"/>
+        <c:axId val="2124022024"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2095526376"/>
+        <c:axId val="2124016232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1814,7 +1826,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
-        <c:crossAx val="2095529352"/>
+        <c:crossAx val="2124022024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1822,7 +1834,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2095529352"/>
+        <c:axId val="2124022024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1869,7 +1881,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2095526376"/>
+        <c:crossAx val="2124016232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1911,15 +1923,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1397000</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:colOff>825500</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>406400</xdr:colOff>
-      <xdr:row>46</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>660400</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1940,16 +1952,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>65</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>762000</xdr:colOff>
-      <xdr:row>88</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>393700</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2293,10 +2305,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:S37"/>
+  <dimension ref="B2:S40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3016,6 +3028,20 @@
       <c r="S37">
         <f t="shared" si="5"/>
         <v>0.22010808804005508</v>
+      </c>
+    </row>
+    <row r="40" spans="2:19">
+      <c r="B40" t="s">
+        <v>19</v>
+      </c>
+      <c r="C40" t="s">
+        <v>20</v>
+      </c>
+      <c r="D40" t="s">
+        <v>21</v>
+      </c>
+      <c r="E40" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>